<commit_message>
Updated model and added LaboratoryFinding profile.
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-ExaminationFinding.xlsx
+++ b/docs/StructureDefinition-ExaminationFinding.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2660" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2659" uniqueCount="422">
   <si>
     <t>Path</t>
   </si>
@@ -512,14 +512,6 @@
     <t>Used for filtering what observations are retrieved and displayed.</t>
   </si>
   <si>
-    <t>&lt;valueCodeableConcept xmlns="http://hl7.org/fhir"&gt;
-  &lt;coding&gt;
-    &lt;system value="http://terminology.hl7.org/CodeSystem/observation-category"/&gt;
-    &lt;code value="exam"/&gt;
-  &lt;/coding&gt;
-&lt;/valueCodeableConcept&gt;</t>
-  </si>
-  <si>
     <t>Codes for high level observation categories.</t>
   </si>
   <si>
@@ -551,13 +543,7 @@
     <t>Knowing what kind of observation is being made is essential to understanding the observation.</t>
   </si>
   <si>
-    <t>example</t>
-  </si>
-  <si>
-    <t>Codes identifying names of simple observations.</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/observation-codes</t>
+    <t>http://aehrc.github.io/genclipr-fhir-ig/ValueSet/AbnormalClinicalFindingCodes</t>
   </si>
   <si>
     <t>Event.code</t>
@@ -924,6 +910,9 @@
   </si>
   <si>
     <t>In some cases, method can impact results and is thus used for determining whether results can be compared or determining significance of results.</t>
+  </si>
+  <si>
+    <t>example</t>
   </si>
   <si>
     <t>Methods for simple observations.</t>
@@ -1275,6 +1264,12 @@
   </si>
   <si>
     <t>*All* code-value and  component.code-component.value pairs need to be taken into account to correctly understand the meaning of the observation.</t>
+  </si>
+  <si>
+    <t>Codes identifying names of simple observations.</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/ValueSet/observation-codes</t>
   </si>
   <si>
     <t>&lt; 363787002 |Observable entity| OR @@ -1535,7 +1530,7 @@
     <col min="22" max="22" width="17.40234375" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.95703125" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="61.72265625" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="58.91015625" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="72.52734375" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="5.8828125" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="20.83984375" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="39.640625" customWidth="true" bestFit="true"/>
@@ -1547,7 +1542,7 @@
     <col min="34" max="34" width="12.71875" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
     <col min="36" max="36" width="26.6875" customWidth="true" bestFit="true"/>
-    <col min="37" max="37" width="242.296875" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="245.77734375" customWidth="true" bestFit="true"/>
     <col min="38" max="38" width="255.0" customWidth="true" bestFit="true"/>
     <col min="39" max="39" width="102.734375" customWidth="true" bestFit="true"/>
     <col min="40" max="40" width="33.046875" customWidth="true" bestFit="true"/>
@@ -3249,7 +3244,7 @@
         <v>45</v>
       </c>
       <c r="R15" t="s" s="2">
-        <v>158</v>
+        <v>45</v>
       </c>
       <c r="S15" t="s" s="2">
         <v>45</v>
@@ -3267,10 +3262,10 @@
         <v>79</v>
       </c>
       <c r="X15" t="s" s="2">
+        <v>158</v>
+      </c>
+      <c r="Y15" t="s" s="2">
         <v>159</v>
-      </c>
-      <c r="Y15" t="s" s="2">
-        <v>160</v>
       </c>
       <c r="Z15" t="s" s="2">
         <v>45</v>
@@ -3312,10 +3307,10 @@
         <v>45</v>
       </c>
       <c r="AM15" t="s" s="2">
+        <v>160</v>
+      </c>
+      <c r="AN15" t="s" s="2">
         <v>161</v>
-      </c>
-      <c r="AN15" t="s" s="2">
-        <v>162</v>
       </c>
       <c r="AO15" t="s" s="2">
         <v>45</v>
@@ -3323,11 +3318,11 @@
     </row>
     <row r="16" hidden="true">
       <c r="A16" t="s" s="2">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s" s="2">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" t="s" s="2">
@@ -3349,16 +3344,16 @@
         <v>153</v>
       </c>
       <c r="K16" t="s" s="2">
+        <v>164</v>
+      </c>
+      <c r="L16" t="s" s="2">
         <v>165</v>
       </c>
-      <c r="L16" t="s" s="2">
+      <c r="M16" t="s" s="2">
         <v>166</v>
       </c>
-      <c r="M16" t="s" s="2">
+      <c r="N16" t="s" s="2">
         <v>167</v>
-      </c>
-      <c r="N16" t="s" s="2">
-        <v>168</v>
       </c>
       <c r="O16" t="s" s="2">
         <v>45</v>
@@ -3383,13 +3378,11 @@
         <v>45</v>
       </c>
       <c r="W16" t="s" s="2">
-        <v>169</v>
-      </c>
-      <c r="X16" t="s" s="2">
-        <v>170</v>
-      </c>
+        <v>144</v>
+      </c>
+      <c r="X16" s="2"/>
       <c r="Y16" t="s" s="2">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="Z16" t="s" s="2">
         <v>45</v>
@@ -3407,7 +3400,7 @@
         <v>45</v>
       </c>
       <c r="AE16" t="s" s="2">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="AF16" t="s" s="2">
         <v>55</v>
@@ -3422,27 +3415,27 @@
         <v>67</v>
       </c>
       <c r="AJ16" t="s" s="2">
+        <v>169</v>
+      </c>
+      <c r="AK16" t="s" s="2">
+        <v>170</v>
+      </c>
+      <c r="AL16" t="s" s="2">
+        <v>171</v>
+      </c>
+      <c r="AM16" t="s" s="2">
         <v>172</v>
       </c>
-      <c r="AK16" t="s" s="2">
+      <c r="AN16" t="s" s="2">
         <v>173</v>
       </c>
-      <c r="AL16" t="s" s="2">
+      <c r="AO16" t="s" s="2">
         <v>174</v>
-      </c>
-      <c r="AM16" t="s" s="2">
-        <v>175</v>
-      </c>
-      <c r="AN16" t="s" s="2">
-        <v>176</v>
-      </c>
-      <c r="AO16" t="s" s="2">
-        <v>177</v>
       </c>
     </row>
     <row r="17" hidden="true">
       <c r="A17" t="s" s="2">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s" s="2">
@@ -3465,19 +3458,19 @@
         <v>56</v>
       </c>
       <c r="J17" t="s" s="2">
+        <v>176</v>
+      </c>
+      <c r="K17" t="s" s="2">
+        <v>177</v>
+      </c>
+      <c r="L17" t="s" s="2">
+        <v>178</v>
+      </c>
+      <c r="M17" t="s" s="2">
         <v>179</v>
       </c>
-      <c r="K17" t="s" s="2">
+      <c r="N17" t="s" s="2">
         <v>180</v>
-      </c>
-      <c r="L17" t="s" s="2">
-        <v>181</v>
-      </c>
-      <c r="M17" t="s" s="2">
-        <v>182</v>
-      </c>
-      <c r="N17" t="s" s="2">
-        <v>183</v>
       </c>
       <c r="O17" t="s" s="2">
         <v>45</v>
@@ -3526,7 +3519,7 @@
         <v>45</v>
       </c>
       <c r="AE17" t="s" s="2">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="AF17" t="s" s="2">
         <v>43</v>
@@ -3541,19 +3534,19 @@
         <v>67</v>
       </c>
       <c r="AJ17" t="s" s="2">
+        <v>181</v>
+      </c>
+      <c r="AK17" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL17" t="s" s="2">
+        <v>182</v>
+      </c>
+      <c r="AM17" t="s" s="2">
+        <v>183</v>
+      </c>
+      <c r="AN17" t="s" s="2">
         <v>184</v>
-      </c>
-      <c r="AK17" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL17" t="s" s="2">
-        <v>185</v>
-      </c>
-      <c r="AM17" t="s" s="2">
-        <v>186</v>
-      </c>
-      <c r="AN17" t="s" s="2">
-        <v>187</v>
       </c>
       <c r="AO17" t="s" s="2">
         <v>45</v>
@@ -3561,7 +3554,7 @@
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
@@ -3584,16 +3577,16 @@
         <v>56</v>
       </c>
       <c r="J18" t="s" s="2">
+        <v>186</v>
+      </c>
+      <c r="K18" t="s" s="2">
+        <v>187</v>
+      </c>
+      <c r="L18" t="s" s="2">
+        <v>188</v>
+      </c>
+      <c r="M18" t="s" s="2">
         <v>189</v>
-      </c>
-      <c r="K18" t="s" s="2">
-        <v>190</v>
-      </c>
-      <c r="L18" t="s" s="2">
-        <v>191</v>
-      </c>
-      <c r="M18" t="s" s="2">
-        <v>192</v>
       </c>
       <c r="N18" s="2"/>
       <c r="O18" t="s" s="2">
@@ -3643,7 +3636,7 @@
         <v>45</v>
       </c>
       <c r="AE18" t="s" s="2">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="AF18" t="s" s="2">
         <v>43</v>
@@ -3664,13 +3657,13 @@
         <v>45</v>
       </c>
       <c r="AL18" t="s" s="2">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="AM18" t="s" s="2">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="AN18" t="s" s="2">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="AO18" t="s" s="2">
         <v>45</v>
@@ -3678,11 +3671,11 @@
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" t="s" s="2">
@@ -3701,19 +3694,19 @@
         <v>56</v>
       </c>
       <c r="J19" t="s" s="2">
+        <v>193</v>
+      </c>
+      <c r="K19" t="s" s="2">
+        <v>194</v>
+      </c>
+      <c r="L19" t="s" s="2">
+        <v>195</v>
+      </c>
+      <c r="M19" t="s" s="2">
         <v>196</v>
       </c>
-      <c r="K19" t="s" s="2">
+      <c r="N19" t="s" s="2">
         <v>197</v>
-      </c>
-      <c r="L19" t="s" s="2">
-        <v>198</v>
-      </c>
-      <c r="M19" t="s" s="2">
-        <v>199</v>
-      </c>
-      <c r="N19" t="s" s="2">
-        <v>200</v>
       </c>
       <c r="O19" t="s" s="2">
         <v>45</v>
@@ -3762,7 +3755,7 @@
         <v>45</v>
       </c>
       <c r="AE19" t="s" s="2">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="AF19" t="s" s="2">
         <v>43</v>
@@ -3777,19 +3770,19 @@
         <v>67</v>
       </c>
       <c r="AJ19" t="s" s="2">
+        <v>198</v>
+      </c>
+      <c r="AK19" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL19" t="s" s="2">
+        <v>199</v>
+      </c>
+      <c r="AM19" t="s" s="2">
+        <v>200</v>
+      </c>
+      <c r="AN19" t="s" s="2">
         <v>201</v>
-      </c>
-      <c r="AK19" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL19" t="s" s="2">
-        <v>202</v>
-      </c>
-      <c r="AM19" t="s" s="2">
-        <v>203</v>
-      </c>
-      <c r="AN19" t="s" s="2">
-        <v>204</v>
       </c>
       <c r="AO19" t="s" s="2">
         <v>45</v>
@@ -3797,11 +3790,11 @@
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" t="s" s="2">
@@ -3820,19 +3813,19 @@
         <v>56</v>
       </c>
       <c r="J20" t="s" s="2">
+        <v>204</v>
+      </c>
+      <c r="K20" t="s" s="2">
+        <v>205</v>
+      </c>
+      <c r="L20" t="s" s="2">
+        <v>206</v>
+      </c>
+      <c r="M20" t="s" s="2">
         <v>207</v>
       </c>
-      <c r="K20" t="s" s="2">
+      <c r="N20" t="s" s="2">
         <v>208</v>
-      </c>
-      <c r="L20" t="s" s="2">
-        <v>209</v>
-      </c>
-      <c r="M20" t="s" s="2">
-        <v>210</v>
-      </c>
-      <c r="N20" t="s" s="2">
-        <v>211</v>
       </c>
       <c r="O20" t="s" s="2">
         <v>45</v>
@@ -3881,7 +3874,7 @@
         <v>45</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="AF20" t="s" s="2">
         <v>43</v>
@@ -3896,19 +3889,19 @@
         <v>67</v>
       </c>
       <c r="AJ20" t="s" s="2">
+        <v>209</v>
+      </c>
+      <c r="AK20" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL20" t="s" s="2">
+        <v>210</v>
+      </c>
+      <c r="AM20" t="s" s="2">
+        <v>211</v>
+      </c>
+      <c r="AN20" t="s" s="2">
         <v>212</v>
-      </c>
-      <c r="AK20" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL20" t="s" s="2">
-        <v>213</v>
-      </c>
-      <c r="AM20" t="s" s="2">
-        <v>214</v>
-      </c>
-      <c r="AN20" t="s" s="2">
-        <v>215</v>
       </c>
       <c r="AO20" t="s" s="2">
         <v>45</v>
@@ -3916,7 +3909,7 @@
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
@@ -3939,16 +3932,16 @@
         <v>56</v>
       </c>
       <c r="J21" t="s" s="2">
+        <v>214</v>
+      </c>
+      <c r="K21" t="s" s="2">
+        <v>215</v>
+      </c>
+      <c r="L21" t="s" s="2">
+        <v>216</v>
+      </c>
+      <c r="M21" t="s" s="2">
         <v>217</v>
-      </c>
-      <c r="K21" t="s" s="2">
-        <v>218</v>
-      </c>
-      <c r="L21" t="s" s="2">
-        <v>219</v>
-      </c>
-      <c r="M21" t="s" s="2">
-        <v>220</v>
       </c>
       <c r="N21" s="2"/>
       <c r="O21" t="s" s="2">
@@ -3998,7 +3991,7 @@
         <v>45</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="AF21" t="s" s="2">
         <v>43</v>
@@ -4019,13 +4012,13 @@
         <v>45</v>
       </c>
       <c r="AL21" t="s" s="2">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="AM21" t="s" s="2">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="AN21" t="s" s="2">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="AO21" t="s" s="2">
         <v>45</v>
@@ -4033,7 +4026,7 @@
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
@@ -4056,17 +4049,17 @@
         <v>56</v>
       </c>
       <c r="J22" t="s" s="2">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="M22" s="2"/>
       <c r="N22" t="s" s="2">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="O22" t="s" s="2">
         <v>45</v>
@@ -4115,7 +4108,7 @@
         <v>45</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="AF22" t="s" s="2">
         <v>43</v>
@@ -4130,19 +4123,19 @@
         <v>67</v>
       </c>
       <c r="AJ22" t="s" s="2">
+        <v>226</v>
+      </c>
+      <c r="AK22" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL22" t="s" s="2">
+        <v>227</v>
+      </c>
+      <c r="AM22" t="s" s="2">
+        <v>228</v>
+      </c>
+      <c r="AN22" t="s" s="2">
         <v>229</v>
-      </c>
-      <c r="AK22" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL22" t="s" s="2">
-        <v>230</v>
-      </c>
-      <c r="AM22" t="s" s="2">
-        <v>231</v>
-      </c>
-      <c r="AN22" t="s" s="2">
-        <v>232</v>
       </c>
       <c r="AO22" t="s" s="2">
         <v>45</v>
@@ -4150,7 +4143,7 @@
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
@@ -4173,19 +4166,19 @@
         <v>56</v>
       </c>
       <c r="J23" t="s" s="2">
+        <v>231</v>
+      </c>
+      <c r="K23" t="s" s="2">
+        <v>232</v>
+      </c>
+      <c r="L23" t="s" s="2">
+        <v>233</v>
+      </c>
+      <c r="M23" t="s" s="2">
         <v>234</v>
       </c>
-      <c r="K23" t="s" s="2">
+      <c r="N23" t="s" s="2">
         <v>235</v>
-      </c>
-      <c r="L23" t="s" s="2">
-        <v>236</v>
-      </c>
-      <c r="M23" t="s" s="2">
-        <v>237</v>
-      </c>
-      <c r="N23" t="s" s="2">
-        <v>238</v>
       </c>
       <c r="O23" t="s" s="2">
         <v>45</v>
@@ -4214,7 +4207,7 @@
       </c>
       <c r="X23" s="2"/>
       <c r="Y23" t="s" s="2">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="Z23" t="s" s="2">
         <v>45</v>
@@ -4232,7 +4225,7 @@
         <v>45</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>43</v>
@@ -4241,7 +4234,7 @@
         <v>55</v>
       </c>
       <c r="AH23" t="s" s="2">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="AI23" t="s" s="2">
         <v>67</v>
@@ -4250,24 +4243,24 @@
         <v>45</v>
       </c>
       <c r="AK23" t="s" s="2">
+        <v>238</v>
+      </c>
+      <c r="AL23" t="s" s="2">
+        <v>239</v>
+      </c>
+      <c r="AM23" t="s" s="2">
+        <v>240</v>
+      </c>
+      <c r="AN23" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO23" t="s" s="2">
         <v>241</v>
-      </c>
-      <c r="AL23" t="s" s="2">
-        <v>242</v>
-      </c>
-      <c r="AM23" t="s" s="2">
-        <v>243</v>
-      </c>
-      <c r="AN23" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO23" t="s" s="2">
-        <v>244</v>
       </c>
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
@@ -4293,16 +4286,16 @@
         <v>153</v>
       </c>
       <c r="K24" t="s" s="2">
+        <v>243</v>
+      </c>
+      <c r="L24" t="s" s="2">
+        <v>244</v>
+      </c>
+      <c r="M24" t="s" s="2">
+        <v>245</v>
+      </c>
+      <c r="N24" t="s" s="2">
         <v>246</v>
-      </c>
-      <c r="L24" t="s" s="2">
-        <v>247</v>
-      </c>
-      <c r="M24" t="s" s="2">
-        <v>248</v>
-      </c>
-      <c r="N24" t="s" s="2">
-        <v>249</v>
       </c>
       <c r="O24" t="s" s="2">
         <v>45</v>
@@ -4327,13 +4320,13 @@
         <v>45</v>
       </c>
       <c r="W24" t="s" s="2">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="X24" t="s" s="2">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="Y24" t="s" s="2">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="Z24" t="s" s="2">
         <v>45</v>
@@ -4351,7 +4344,7 @@
         <v>45</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>43</v>
@@ -4360,7 +4353,7 @@
         <v>55</v>
       </c>
       <c r="AH24" t="s" s="2">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="AI24" t="s" s="2">
         <v>67</v>
@@ -4375,7 +4368,7 @@
         <v>98</v>
       </c>
       <c r="AM24" t="s" s="2">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="AN24" t="s" s="2">
         <v>45</v>
@@ -4386,11 +4379,11 @@
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" t="s" s="2">
@@ -4412,16 +4405,16 @@
         <v>153</v>
       </c>
       <c r="K25" t="s" s="2">
+        <v>254</v>
+      </c>
+      <c r="L25" t="s" s="2">
+        <v>255</v>
+      </c>
+      <c r="M25" t="s" s="2">
+        <v>256</v>
+      </c>
+      <c r="N25" t="s" s="2">
         <v>257</v>
-      </c>
-      <c r="L25" t="s" s="2">
-        <v>258</v>
-      </c>
-      <c r="M25" t="s" s="2">
-        <v>259</v>
-      </c>
-      <c r="N25" t="s" s="2">
-        <v>260</v>
       </c>
       <c r="O25" t="s" s="2">
         <v>45</v>
@@ -4446,13 +4439,13 @@
         <v>45</v>
       </c>
       <c r="W25" t="s" s="2">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="X25" t="s" s="2">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="Y25" t="s" s="2">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="Z25" t="s" s="2">
         <v>45</v>
@@ -4470,7 +4463,7 @@
         <v>45</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>43</v>
@@ -4488,24 +4481,24 @@
         <v>45</v>
       </c>
       <c r="AK25" t="s" s="2">
+        <v>260</v>
+      </c>
+      <c r="AL25" t="s" s="2">
+        <v>261</v>
+      </c>
+      <c r="AM25" t="s" s="2">
+        <v>262</v>
+      </c>
+      <c r="AN25" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO25" t="s" s="2">
         <v>263</v>
-      </c>
-      <c r="AL25" t="s" s="2">
-        <v>264</v>
-      </c>
-      <c r="AM25" t="s" s="2">
-        <v>265</v>
-      </c>
-      <c r="AN25" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO25" t="s" s="2">
-        <v>266</v>
       </c>
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
@@ -4528,19 +4521,19 @@
         <v>45</v>
       </c>
       <c r="J26" t="s" s="2">
+        <v>265</v>
+      </c>
+      <c r="K26" t="s" s="2">
+        <v>266</v>
+      </c>
+      <c r="L26" t="s" s="2">
+        <v>267</v>
+      </c>
+      <c r="M26" t="s" s="2">
         <v>268</v>
       </c>
-      <c r="K26" t="s" s="2">
+      <c r="N26" t="s" s="2">
         <v>269</v>
-      </c>
-      <c r="L26" t="s" s="2">
-        <v>270</v>
-      </c>
-      <c r="M26" t="s" s="2">
-        <v>271</v>
-      </c>
-      <c r="N26" t="s" s="2">
-        <v>272</v>
       </c>
       <c r="O26" t="s" s="2">
         <v>45</v>
@@ -4589,7 +4582,7 @@
         <v>45</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="AF26" t="s" s="2">
         <v>43</v>
@@ -4610,10 +4603,10 @@
         <v>45</v>
       </c>
       <c r="AL26" t="s" s="2">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="AM26" t="s" s="2">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="AN26" t="s" s="2">
         <v>45</v>
@@ -4624,7 +4617,7 @@
     </row>
     <row r="27">
       <c r="A27" t="s" s="2">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
@@ -4650,13 +4643,13 @@
         <v>153</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="M27" t="s" s="2">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="N27" s="2"/>
       <c r="O27" t="s" s="2">
@@ -4686,7 +4679,7 @@
       </c>
       <c r="X27" s="2"/>
       <c r="Y27" t="s" s="2">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="Z27" t="s" s="2">
         <v>45</v>
@@ -4704,7 +4697,7 @@
         <v>45</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>43</v>
@@ -4722,24 +4715,24 @@
         <v>45</v>
       </c>
       <c r="AK27" t="s" s="2">
+        <v>277</v>
+      </c>
+      <c r="AL27" t="s" s="2">
+        <v>278</v>
+      </c>
+      <c r="AM27" t="s" s="2">
+        <v>279</v>
+      </c>
+      <c r="AN27" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO27" t="s" s="2">
         <v>280</v>
-      </c>
-      <c r="AL27" t="s" s="2">
-        <v>281</v>
-      </c>
-      <c r="AM27" t="s" s="2">
-        <v>282</v>
-      </c>
-      <c r="AN27" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO27" t="s" s="2">
-        <v>283</v>
       </c>
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -4765,16 +4758,16 @@
         <v>153</v>
       </c>
       <c r="K28" t="s" s="2">
+        <v>282</v>
+      </c>
+      <c r="L28" t="s" s="2">
+        <v>283</v>
+      </c>
+      <c r="M28" t="s" s="2">
+        <v>284</v>
+      </c>
+      <c r="N28" t="s" s="2">
         <v>285</v>
-      </c>
-      <c r="L28" t="s" s="2">
-        <v>286</v>
-      </c>
-      <c r="M28" t="s" s="2">
-        <v>287</v>
-      </c>
-      <c r="N28" t="s" s="2">
-        <v>288</v>
       </c>
       <c r="O28" t="s" s="2">
         <v>45</v>
@@ -4799,13 +4792,13 @@
         <v>45</v>
       </c>
       <c r="W28" t="s" s="2">
-        <v>169</v>
+        <v>286</v>
       </c>
       <c r="X28" t="s" s="2">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="Y28" t="s" s="2">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="Z28" t="s" s="2">
         <v>45</v>
@@ -4823,7 +4816,7 @@
         <v>45</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>43</v>
@@ -4844,10 +4837,10 @@
         <v>45</v>
       </c>
       <c r="AL28" t="s" s="2">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="AM28" t="s" s="2">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="AN28" t="s" s="2">
         <v>45</v>
@@ -4858,7 +4851,7 @@
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -4881,16 +4874,16 @@
         <v>45</v>
       </c>
       <c r="J29" t="s" s="2">
+        <v>292</v>
+      </c>
+      <c r="K29" t="s" s="2">
+        <v>293</v>
+      </c>
+      <c r="L29" t="s" s="2">
         <v>294</v>
       </c>
-      <c r="K29" t="s" s="2">
+      <c r="M29" t="s" s="2">
         <v>295</v>
-      </c>
-      <c r="L29" t="s" s="2">
-        <v>296</v>
-      </c>
-      <c r="M29" t="s" s="2">
-        <v>297</v>
       </c>
       <c r="N29" s="2"/>
       <c r="O29" t="s" s="2">
@@ -4940,7 +4933,7 @@
         <v>45</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>43</v>
@@ -4958,24 +4951,24 @@
         <v>45</v>
       </c>
       <c r="AK29" t="s" s="2">
+        <v>296</v>
+      </c>
+      <c r="AL29" t="s" s="2">
+        <v>297</v>
+      </c>
+      <c r="AM29" t="s" s="2">
         <v>298</v>
       </c>
-      <c r="AL29" t="s" s="2">
+      <c r="AN29" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO29" t="s" s="2">
         <v>299</v>
-      </c>
-      <c r="AM29" t="s" s="2">
-        <v>300</v>
-      </c>
-      <c r="AN29" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO29" t="s" s="2">
-        <v>301</v>
       </c>
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -4998,16 +4991,16 @@
         <v>45</v>
       </c>
       <c r="J30" t="s" s="2">
+        <v>301</v>
+      </c>
+      <c r="K30" t="s" s="2">
+        <v>302</v>
+      </c>
+      <c r="L30" t="s" s="2">
         <v>303</v>
       </c>
-      <c r="K30" t="s" s="2">
+      <c r="M30" t="s" s="2">
         <v>304</v>
-      </c>
-      <c r="L30" t="s" s="2">
-        <v>305</v>
-      </c>
-      <c r="M30" t="s" s="2">
-        <v>306</v>
       </c>
       <c r="N30" s="2"/>
       <c r="O30" t="s" s="2">
@@ -5057,7 +5050,7 @@
         <v>45</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>43</v>
@@ -5075,24 +5068,24 @@
         <v>45</v>
       </c>
       <c r="AK30" t="s" s="2">
+        <v>305</v>
+      </c>
+      <c r="AL30" t="s" s="2">
+        <v>306</v>
+      </c>
+      <c r="AM30" t="s" s="2">
         <v>307</v>
       </c>
-      <c r="AL30" t="s" s="2">
+      <c r="AN30" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO30" t="s" s="2">
         <v>308</v>
-      </c>
-      <c r="AM30" t="s" s="2">
-        <v>309</v>
-      </c>
-      <c r="AN30" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO30" t="s" s="2">
-        <v>310</v>
       </c>
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -5115,19 +5108,19 @@
         <v>45</v>
       </c>
       <c r="J31" t="s" s="2">
+        <v>310</v>
+      </c>
+      <c r="K31" t="s" s="2">
+        <v>311</v>
+      </c>
+      <c r="L31" t="s" s="2">
         <v>312</v>
       </c>
-      <c r="K31" t="s" s="2">
+      <c r="M31" t="s" s="2">
         <v>313</v>
       </c>
-      <c r="L31" t="s" s="2">
+      <c r="N31" t="s" s="2">
         <v>314</v>
-      </c>
-      <c r="M31" t="s" s="2">
-        <v>315</v>
-      </c>
-      <c r="N31" t="s" s="2">
-        <v>316</v>
       </c>
       <c r="O31" t="s" s="2">
         <v>45</v>
@@ -5176,7 +5169,7 @@
         <v>45</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>43</v>
@@ -5188,19 +5181,19 @@
         <v>45</v>
       </c>
       <c r="AI31" t="s" s="2">
+        <v>315</v>
+      </c>
+      <c r="AJ31" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK31" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL31" t="s" s="2">
+        <v>316</v>
+      </c>
+      <c r="AM31" t="s" s="2">
         <v>317</v>
-      </c>
-      <c r="AJ31" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AK31" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL31" t="s" s="2">
-        <v>318</v>
-      </c>
-      <c r="AM31" t="s" s="2">
-        <v>319</v>
       </c>
       <c r="AN31" t="s" s="2">
         <v>45</v>
@@ -5211,7 +5204,7 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
@@ -5237,10 +5230,10 @@
         <v>57</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
@@ -5291,7 +5284,7 @@
         <v>45</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>43</v>
@@ -5315,7 +5308,7 @@
         <v>45</v>
       </c>
       <c r="AM32" t="s" s="2">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="AN32" t="s" s="2">
         <v>45</v>
@@ -5326,7 +5319,7 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
@@ -5355,7 +5348,7 @@
         <v>102</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="M33" t="s" s="2">
         <v>104</v>
@@ -5408,7 +5401,7 @@
         <v>45</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>43</v>
@@ -5432,7 +5425,7 @@
         <v>45</v>
       </c>
       <c r="AM33" t="s" s="2">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="AN33" t="s" s="2">
         <v>45</v>
@@ -5443,11 +5436,11 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" t="s" s="2">
@@ -5469,10 +5462,10 @@
         <v>101</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="M34" t="s" s="2">
         <v>104</v>
@@ -5527,7 +5520,7 @@
         <v>45</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>43</v>
@@ -5562,7 +5555,7 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -5585,13 +5578,13 @@
         <v>45</v>
       </c>
       <c r="J35" t="s" s="2">
+        <v>332</v>
+      </c>
+      <c r="K35" t="s" s="2">
+        <v>333</v>
+      </c>
+      <c r="L35" t="s" s="2">
         <v>334</v>
-      </c>
-      <c r="K35" t="s" s="2">
-        <v>335</v>
-      </c>
-      <c r="L35" t="s" s="2">
-        <v>336</v>
       </c>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
@@ -5642,7 +5635,7 @@
         <v>45</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>43</v>
@@ -5651,7 +5644,7 @@
         <v>55</v>
       </c>
       <c r="AH35" t="s" s="2">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="AI35" t="s" s="2">
         <v>67</v>
@@ -5663,10 +5656,10 @@
         <v>45</v>
       </c>
       <c r="AL35" t="s" s="2">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="AM35" t="s" s="2">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="AN35" t="s" s="2">
         <v>45</v>
@@ -5677,7 +5670,7 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -5700,13 +5693,13 @@
         <v>45</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
@@ -5757,7 +5750,7 @@
         <v>45</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>43</v>
@@ -5766,7 +5759,7 @@
         <v>55</v>
       </c>
       <c r="AH36" t="s" s="2">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="AI36" t="s" s="2">
         <v>67</v>
@@ -5778,10 +5771,10 @@
         <v>45</v>
       </c>
       <c r="AL36" t="s" s="2">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="AM36" t="s" s="2">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="AN36" t="s" s="2">
         <v>45</v>
@@ -5792,7 +5785,7 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -5818,16 +5811,16 @@
         <v>153</v>
       </c>
       <c r="K37" t="s" s="2">
+        <v>343</v>
+      </c>
+      <c r="L37" t="s" s="2">
+        <v>344</v>
+      </c>
+      <c r="M37" t="s" s="2">
         <v>345</v>
       </c>
-      <c r="L37" t="s" s="2">
+      <c r="N37" t="s" s="2">
         <v>346</v>
-      </c>
-      <c r="M37" t="s" s="2">
-        <v>347</v>
-      </c>
-      <c r="N37" t="s" s="2">
-        <v>348</v>
       </c>
       <c r="O37" t="s" s="2">
         <v>45</v>
@@ -5855,10 +5848,10 @@
         <v>79</v>
       </c>
       <c r="X37" t="s" s="2">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="Y37" t="s" s="2">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="Z37" t="s" s="2">
         <v>45</v>
@@ -5876,7 +5869,7 @@
         <v>45</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>43</v>
@@ -5894,13 +5887,13 @@
         <v>45</v>
       </c>
       <c r="AK37" t="s" s="2">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="AL37" t="s" s="2">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="AM37" t="s" s="2">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="AN37" t="s" s="2">
         <v>45</v>
@@ -5911,7 +5904,7 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5937,16 +5930,16 @@
         <v>153</v>
       </c>
       <c r="K38" t="s" s="2">
+        <v>352</v>
+      </c>
+      <c r="L38" t="s" s="2">
+        <v>353</v>
+      </c>
+      <c r="M38" t="s" s="2">
         <v>354</v>
       </c>
-      <c r="L38" t="s" s="2">
+      <c r="N38" t="s" s="2">
         <v>355</v>
-      </c>
-      <c r="M38" t="s" s="2">
-        <v>356</v>
-      </c>
-      <c r="N38" t="s" s="2">
-        <v>357</v>
       </c>
       <c r="O38" t="s" s="2">
         <v>45</v>
@@ -5971,13 +5964,13 @@
         <v>45</v>
       </c>
       <c r="W38" t="s" s="2">
-        <v>169</v>
+        <v>286</v>
       </c>
       <c r="X38" t="s" s="2">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="Y38" t="s" s="2">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="Z38" t="s" s="2">
         <v>45</v>
@@ -5995,7 +5988,7 @@
         <v>45</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>43</v>
@@ -6013,13 +6006,13 @@
         <v>45</v>
       </c>
       <c r="AK38" t="s" s="2">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="AM38" t="s" s="2">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="AN38" t="s" s="2">
         <v>45</v>
@@ -6030,7 +6023,7 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -6053,17 +6046,17 @@
         <v>45</v>
       </c>
       <c r="J39" t="s" s="2">
+        <v>359</v>
+      </c>
+      <c r="K39" t="s" s="2">
+        <v>360</v>
+      </c>
+      <c r="L39" t="s" s="2">
         <v>361</v>
-      </c>
-      <c r="K39" t="s" s="2">
-        <v>362</v>
-      </c>
-      <c r="L39" t="s" s="2">
-        <v>363</v>
       </c>
       <c r="M39" s="2"/>
       <c r="N39" t="s" s="2">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="O39" t="s" s="2">
         <v>45</v>
@@ -6112,7 +6105,7 @@
         <v>45</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>43</v>
@@ -6136,7 +6129,7 @@
         <v>45</v>
       </c>
       <c r="AM39" t="s" s="2">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="AN39" t="s" s="2">
         <v>45</v>
@@ -6147,7 +6140,7 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -6173,10 +6166,10 @@
         <v>57</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
@@ -6227,7 +6220,7 @@
         <v>45</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>43</v>
@@ -6248,10 +6241,10 @@
         <v>45</v>
       </c>
       <c r="AL40" t="s" s="2">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="AM40" t="s" s="2">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="AN40" t="s" s="2">
         <v>45</v>
@@ -6262,7 +6255,7 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -6285,16 +6278,16 @@
         <v>56</v>
       </c>
       <c r="J41" t="s" s="2">
+        <v>369</v>
+      </c>
+      <c r="K41" t="s" s="2">
+        <v>370</v>
+      </c>
+      <c r="L41" t="s" s="2">
         <v>371</v>
       </c>
-      <c r="K41" t="s" s="2">
+      <c r="M41" t="s" s="2">
         <v>372</v>
-      </c>
-      <c r="L41" t="s" s="2">
-        <v>373</v>
-      </c>
-      <c r="M41" t="s" s="2">
-        <v>374</v>
       </c>
       <c r="N41" s="2"/>
       <c r="O41" t="s" s="2">
@@ -6344,7 +6337,7 @@
         <v>45</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>43</v>
@@ -6365,10 +6358,10 @@
         <v>45</v>
       </c>
       <c r="AL41" t="s" s="2">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="AM41" t="s" s="2">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="AN41" t="s" s="2">
         <v>45</v>
@@ -6379,7 +6372,7 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
@@ -6402,16 +6395,16 @@
         <v>56</v>
       </c>
       <c r="J42" t="s" s="2">
+        <v>376</v>
+      </c>
+      <c r="K42" t="s" s="2">
+        <v>377</v>
+      </c>
+      <c r="L42" t="s" s="2">
         <v>378</v>
       </c>
-      <c r="K42" t="s" s="2">
+      <c r="M42" t="s" s="2">
         <v>379</v>
-      </c>
-      <c r="L42" t="s" s="2">
-        <v>380</v>
-      </c>
-      <c r="M42" t="s" s="2">
-        <v>381</v>
       </c>
       <c r="N42" s="2"/>
       <c r="O42" t="s" s="2">
@@ -6461,7 +6454,7 @@
         <v>45</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>43</v>
@@ -6482,10 +6475,10 @@
         <v>45</v>
       </c>
       <c r="AL42" t="s" s="2">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="AM42" t="s" s="2">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="AN42" t="s" s="2">
         <v>45</v>
@@ -6496,7 +6489,7 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
@@ -6519,19 +6512,19 @@
         <v>56</v>
       </c>
       <c r="J43" t="s" s="2">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="K43" t="s" s="2">
+        <v>382</v>
+      </c>
+      <c r="L43" t="s" s="2">
+        <v>383</v>
+      </c>
+      <c r="M43" t="s" s="2">
         <v>384</v>
       </c>
-      <c r="L43" t="s" s="2">
+      <c r="N43" t="s" s="2">
         <v>385</v>
-      </c>
-      <c r="M43" t="s" s="2">
-        <v>386</v>
-      </c>
-      <c r="N43" t="s" s="2">
-        <v>387</v>
       </c>
       <c r="O43" t="s" s="2">
         <v>45</v>
@@ -6568,19 +6561,19 @@
         <v>45</v>
       </c>
       <c r="AA43" t="s" s="2">
+        <v>386</v>
+      </c>
+      <c r="AB43" t="s" s="2">
+        <v>387</v>
+      </c>
+      <c r="AC43" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD43" t="s" s="2">
         <v>388</v>
       </c>
-      <c r="AB43" t="s" s="2">
-        <v>389</v>
-      </c>
-      <c r="AC43" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AD43" t="s" s="2">
-        <v>390</v>
-      </c>
       <c r="AE43" t="s" s="2">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>43</v>
@@ -6601,10 +6594,10 @@
         <v>45</v>
       </c>
       <c r="AL43" t="s" s="2">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="AM43" t="s" s="2">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="AN43" t="s" s="2">
         <v>45</v>
@@ -6615,7 +6608,7 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -6641,10 +6634,10 @@
         <v>57</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="M44" s="2"/>
       <c r="N44" s="2"/>
@@ -6695,7 +6688,7 @@
         <v>45</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>43</v>
@@ -6719,7 +6712,7 @@
         <v>45</v>
       </c>
       <c r="AM44" t="s" s="2">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="AN44" t="s" s="2">
         <v>45</v>
@@ -6730,7 +6723,7 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -6759,7 +6752,7 @@
         <v>102</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="M45" t="s" s="2">
         <v>104</v>
@@ -6812,7 +6805,7 @@
         <v>45</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="AF45" t="s" s="2">
         <v>43</v>
@@ -6836,7 +6829,7 @@
         <v>45</v>
       </c>
       <c r="AM45" t="s" s="2">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="AN45" t="s" s="2">
         <v>45</v>
@@ -6847,11 +6840,11 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" t="s" s="2">
@@ -6873,10 +6866,10 @@
         <v>101</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="M46" t="s" s="2">
         <v>104</v>
@@ -6931,7 +6924,7 @@
         <v>45</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>43</v>
@@ -6966,7 +6959,7 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
@@ -6992,16 +6985,16 @@
         <v>153</v>
       </c>
       <c r="K47" t="s" s="2">
+        <v>395</v>
+      </c>
+      <c r="L47" t="s" s="2">
+        <v>396</v>
+      </c>
+      <c r="M47" t="s" s="2">
         <v>397</v>
       </c>
-      <c r="L47" t="s" s="2">
-        <v>398</v>
-      </c>
-      <c r="M47" t="s" s="2">
-        <v>399</v>
-      </c>
       <c r="N47" t="s" s="2">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="O47" t="s" s="2">
         <v>45</v>
@@ -7026,13 +7019,13 @@
         <v>45</v>
       </c>
       <c r="W47" t="s" s="2">
-        <v>169</v>
+        <v>286</v>
       </c>
       <c r="X47" t="s" s="2">
-        <v>170</v>
+        <v>398</v>
       </c>
       <c r="Y47" t="s" s="2">
-        <v>171</v>
+        <v>399</v>
       </c>
       <c r="Z47" t="s" s="2">
         <v>45</v>
@@ -7050,7 +7043,7 @@
         <v>45</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>55</v>
@@ -7071,13 +7064,13 @@
         <v>400</v>
       </c>
       <c r="AL47" t="s" s="2">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="AM47" t="s" s="2">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="AN47" t="s" s="2">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="AO47" t="s" s="2">
         <v>45</v>
@@ -7108,19 +7101,19 @@
         <v>56</v>
       </c>
       <c r="J48" t="s" s="2">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="K48" t="s" s="2">
         <v>402</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="M48" t="s" s="2">
         <v>403</v>
       </c>
       <c r="N48" t="s" s="2">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="O48" t="s" s="2">
         <v>45</v>
@@ -7190,16 +7183,16 @@
         <v>404</v>
       </c>
       <c r="AL48" t="s" s="2">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="AM48" t="s" s="2">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="AN48" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO48" t="s" s="2">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="49" hidden="true">
@@ -7239,7 +7232,7 @@
         <v>408</v>
       </c>
       <c r="N49" t="s" s="2">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="O49" t="s" s="2">
         <v>45</v>
@@ -7264,13 +7257,13 @@
         <v>45</v>
       </c>
       <c r="W49" t="s" s="2">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="X49" t="s" s="2">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="Y49" t="s" s="2">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="Z49" t="s" s="2">
         <v>45</v>
@@ -7297,7 +7290,7 @@
         <v>55</v>
       </c>
       <c r="AH49" t="s" s="2">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="AI49" t="s" s="2">
         <v>67</v>
@@ -7312,7 +7305,7 @@
         <v>98</v>
       </c>
       <c r="AM49" t="s" s="2">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="AN49" t="s" s="2">
         <v>45</v>
@@ -7327,7 +7320,7 @@
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" t="s" s="2">
@@ -7349,16 +7342,16 @@
         <v>153</v>
       </c>
       <c r="K50" t="s" s="2">
+        <v>254</v>
+      </c>
+      <c r="L50" t="s" s="2">
+        <v>255</v>
+      </c>
+      <c r="M50" t="s" s="2">
+        <v>256</v>
+      </c>
+      <c r="N50" t="s" s="2">
         <v>257</v>
-      </c>
-      <c r="L50" t="s" s="2">
-        <v>258</v>
-      </c>
-      <c r="M50" t="s" s="2">
-        <v>259</v>
-      </c>
-      <c r="N50" t="s" s="2">
-        <v>260</v>
       </c>
       <c r="O50" t="s" s="2">
         <v>45</v>
@@ -7383,13 +7376,13 @@
         <v>45</v>
       </c>
       <c r="W50" t="s" s="2">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="X50" t="s" s="2">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="Y50" t="s" s="2">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="Z50" t="s" s="2">
         <v>45</v>
@@ -7425,19 +7418,19 @@
         <v>45</v>
       </c>
       <c r="AK50" t="s" s="2">
+        <v>260</v>
+      </c>
+      <c r="AL50" t="s" s="2">
+        <v>261</v>
+      </c>
+      <c r="AM50" t="s" s="2">
+        <v>262</v>
+      </c>
+      <c r="AN50" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO50" t="s" s="2">
         <v>263</v>
-      </c>
-      <c r="AL50" t="s" s="2">
-        <v>264</v>
-      </c>
-      <c r="AM50" t="s" s="2">
-        <v>265</v>
-      </c>
-      <c r="AN50" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO50" t="s" s="2">
-        <v>266</v>
       </c>
     </row>
     <row r="51" hidden="true">
@@ -7474,10 +7467,10 @@
         <v>412</v>
       </c>
       <c r="M51" t="s" s="2">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="N51" t="s" s="2">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="O51" t="s" s="2">
         <v>45</v>
@@ -7547,10 +7540,10 @@
         <v>45</v>
       </c>
       <c r="AL51" t="s" s="2">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="AM51" t="s" s="2">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="AN51" t="s" s="2">
         <v>45</v>
@@ -7561,7 +7554,7 @@
     </row>
     <row r="52">
       <c r="A52" t="s" s="2">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B52" t="s" s="2">
         <v>413</v>
@@ -7586,19 +7579,19 @@
         <v>56</v>
       </c>
       <c r="J52" t="s" s="2">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="K52" t="s" s="2">
+        <v>382</v>
+      </c>
+      <c r="L52" t="s" s="2">
+        <v>383</v>
+      </c>
+      <c r="M52" t="s" s="2">
         <v>384</v>
       </c>
-      <c r="L52" t="s" s="2">
+      <c r="N52" t="s" s="2">
         <v>385</v>
-      </c>
-      <c r="M52" t="s" s="2">
-        <v>386</v>
-      </c>
-      <c r="N52" t="s" s="2">
-        <v>387</v>
       </c>
       <c r="O52" t="s" s="2">
         <v>45</v>
@@ -7647,7 +7640,7 @@
         <v>45</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>43</v>
@@ -7668,10 +7661,10 @@
         <v>45</v>
       </c>
       <c r="AL52" t="s" s="2">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="AM52" t="s" s="2">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="AN52" t="s" s="2">
         <v>45</v>
@@ -7682,7 +7675,7 @@
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
@@ -7708,10 +7701,10 @@
         <v>57</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="M53" s="2"/>
       <c r="N53" s="2"/>
@@ -7762,7 +7755,7 @@
         <v>45</v>
       </c>
       <c r="AE53" t="s" s="2">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="AF53" t="s" s="2">
         <v>43</v>
@@ -7786,7 +7779,7 @@
         <v>45</v>
       </c>
       <c r="AM53" t="s" s="2">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="AN53" t="s" s="2">
         <v>45</v>
@@ -7797,7 +7790,7 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" t="s" s="2">
@@ -7826,7 +7819,7 @@
         <v>102</v>
       </c>
       <c r="L54" t="s" s="2">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="M54" t="s" s="2">
         <v>104</v>
@@ -7879,7 +7872,7 @@
         <v>45</v>
       </c>
       <c r="AE54" t="s" s="2">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="AF54" t="s" s="2">
         <v>43</v>
@@ -7903,7 +7896,7 @@
         <v>45</v>
       </c>
       <c r="AM54" t="s" s="2">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="AN54" t="s" s="2">
         <v>45</v>
@@ -7914,11 +7907,11 @@
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" t="s" s="2">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" t="s" s="2">
@@ -7940,10 +7933,10 @@
         <v>101</v>
       </c>
       <c r="K55" t="s" s="2">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="L55" t="s" s="2">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="M55" t="s" s="2">
         <v>104</v>
@@ -7998,7 +7991,7 @@
         <v>45</v>
       </c>
       <c r="AE55" t="s" s="2">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="AF55" t="s" s="2">
         <v>43</v>
@@ -8033,7 +8026,7 @@
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" t="s" s="2">
@@ -8059,16 +8052,16 @@
         <v>153</v>
       </c>
       <c r="K56" t="s" s="2">
+        <v>395</v>
+      </c>
+      <c r="L56" t="s" s="2">
+        <v>396</v>
+      </c>
+      <c r="M56" t="s" s="2">
         <v>397</v>
       </c>
-      <c r="L56" t="s" s="2">
-        <v>398</v>
-      </c>
-      <c r="M56" t="s" s="2">
-        <v>399</v>
-      </c>
       <c r="N56" t="s" s="2">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="O56" t="s" s="2">
         <v>45</v>
@@ -8093,13 +8086,13 @@
         <v>45</v>
       </c>
       <c r="W56" t="s" s="2">
-        <v>169</v>
+        <v>286</v>
       </c>
       <c r="X56" t="s" s="2">
-        <v>170</v>
+        <v>398</v>
       </c>
       <c r="Y56" t="s" s="2">
-        <v>171</v>
+        <v>399</v>
       </c>
       <c r="Z56" t="s" s="2">
         <v>45</v>
@@ -8117,7 +8110,7 @@
         <v>45</v>
       </c>
       <c r="AE56" t="s" s="2">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="AF56" t="s" s="2">
         <v>55</v>
@@ -8138,13 +8131,13 @@
         <v>400</v>
       </c>
       <c r="AL56" t="s" s="2">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="AM56" t="s" s="2">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="AN56" t="s" s="2">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="AO56" t="s" s="2">
         <v>45</v>
@@ -8181,13 +8174,13 @@
         <v>402</v>
       </c>
       <c r="L57" t="s" s="2">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="M57" t="s" s="2">
         <v>403</v>
       </c>
       <c r="N57" t="s" s="2">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="O57" t="s" s="2">
         <v>45</v>
@@ -8255,16 +8248,16 @@
         <v>404</v>
       </c>
       <c r="AL57" t="s" s="2">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="AM57" t="s" s="2">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="AN57" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO57" t="s" s="2">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="58" hidden="true">
@@ -8300,13 +8293,13 @@
         <v>402</v>
       </c>
       <c r="L58" t="s" s="2">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="M58" t="s" s="2">
         <v>403</v>
       </c>
       <c r="N58" t="s" s="2">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="O58" t="s" s="2">
         <v>45</v>
@@ -8374,16 +8367,16 @@
         <v>404</v>
       </c>
       <c r="AL58" t="s" s="2">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="AM58" t="s" s="2">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="AN58" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO58" t="s" s="2">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="59" hidden="true">
@@ -8423,7 +8416,7 @@
         <v>408</v>
       </c>
       <c r="N59" t="s" s="2">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="O59" t="s" s="2">
         <v>45</v>
@@ -8448,13 +8441,13 @@
         <v>45</v>
       </c>
       <c r="W59" t="s" s="2">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="X59" t="s" s="2">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="Y59" t="s" s="2">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="Z59" t="s" s="2">
         <v>45</v>
@@ -8481,7 +8474,7 @@
         <v>55</v>
       </c>
       <c r="AH59" t="s" s="2">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="AI59" t="s" s="2">
         <v>67</v>
@@ -8496,7 +8489,7 @@
         <v>98</v>
       </c>
       <c r="AM59" t="s" s="2">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="AN59" t="s" s="2">
         <v>45</v>
@@ -8511,7 +8504,7 @@
       </c>
       <c r="B60" s="2"/>
       <c r="C60" t="s" s="2">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D60" s="2"/>
       <c r="E60" t="s" s="2">
@@ -8533,16 +8526,16 @@
         <v>153</v>
       </c>
       <c r="K60" t="s" s="2">
+        <v>254</v>
+      </c>
+      <c r="L60" t="s" s="2">
+        <v>255</v>
+      </c>
+      <c r="M60" t="s" s="2">
+        <v>256</v>
+      </c>
+      <c r="N60" t="s" s="2">
         <v>257</v>
-      </c>
-      <c r="L60" t="s" s="2">
-        <v>258</v>
-      </c>
-      <c r="M60" t="s" s="2">
-        <v>259</v>
-      </c>
-      <c r="N60" t="s" s="2">
-        <v>260</v>
       </c>
       <c r="O60" t="s" s="2">
         <v>45</v>
@@ -8567,13 +8560,13 @@
         <v>45</v>
       </c>
       <c r="W60" t="s" s="2">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="X60" t="s" s="2">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="Y60" t="s" s="2">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="Z60" t="s" s="2">
         <v>45</v>
@@ -8609,19 +8602,19 @@
         <v>45</v>
       </c>
       <c r="AK60" t="s" s="2">
+        <v>260</v>
+      </c>
+      <c r="AL60" t="s" s="2">
+        <v>261</v>
+      </c>
+      <c r="AM60" t="s" s="2">
+        <v>262</v>
+      </c>
+      <c r="AN60" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO60" t="s" s="2">
         <v>263</v>
-      </c>
-      <c r="AL60" t="s" s="2">
-        <v>264</v>
-      </c>
-      <c r="AM60" t="s" s="2">
-        <v>265</v>
-      </c>
-      <c r="AN60" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO60" t="s" s="2">
-        <v>266</v>
       </c>
     </row>
     <row r="61" hidden="true">
@@ -8658,10 +8651,10 @@
         <v>412</v>
       </c>
       <c r="M61" t="s" s="2">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="N61" t="s" s="2">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="O61" t="s" s="2">
         <v>45</v>
@@ -8731,10 +8724,10 @@
         <v>45</v>
       </c>
       <c r="AL61" t="s" s="2">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="AM61" t="s" s="2">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="AN61" t="s" s="2">
         <v>45</v>
@@ -8745,7 +8738,7 @@
     </row>
     <row r="62">
       <c r="A62" t="s" s="2">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B62" t="s" s="2">
         <v>419</v>
@@ -8770,19 +8763,19 @@
         <v>56</v>
       </c>
       <c r="J62" t="s" s="2">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="K62" t="s" s="2">
+        <v>382</v>
+      </c>
+      <c r="L62" t="s" s="2">
+        <v>383</v>
+      </c>
+      <c r="M62" t="s" s="2">
         <v>384</v>
       </c>
-      <c r="L62" t="s" s="2">
+      <c r="N62" t="s" s="2">
         <v>385</v>
-      </c>
-      <c r="M62" t="s" s="2">
-        <v>386</v>
-      </c>
-      <c r="N62" t="s" s="2">
-        <v>387</v>
       </c>
       <c r="O62" t="s" s="2">
         <v>45</v>
@@ -8831,7 +8824,7 @@
         <v>45</v>
       </c>
       <c r="AE62" t="s" s="2">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="AF62" t="s" s="2">
         <v>43</v>
@@ -8852,10 +8845,10 @@
         <v>45</v>
       </c>
       <c r="AL62" t="s" s="2">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="AM62" t="s" s="2">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="AN62" t="s" s="2">
         <v>45</v>
@@ -8866,7 +8859,7 @@
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" t="s" s="2">
@@ -8892,10 +8885,10 @@
         <v>57</v>
       </c>
       <c r="K63" t="s" s="2">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="L63" t="s" s="2">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="M63" s="2"/>
       <c r="N63" s="2"/>
@@ -8946,7 +8939,7 @@
         <v>45</v>
       </c>
       <c r="AE63" t="s" s="2">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="AF63" t="s" s="2">
         <v>43</v>
@@ -8970,7 +8963,7 @@
         <v>45</v>
       </c>
       <c r="AM63" t="s" s="2">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="AN63" t="s" s="2">
         <v>45</v>
@@ -8981,7 +8974,7 @@
     </row>
     <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" t="s" s="2">
@@ -9010,7 +9003,7 @@
         <v>102</v>
       </c>
       <c r="L64" t="s" s="2">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="M64" t="s" s="2">
         <v>104</v>
@@ -9063,7 +9056,7 @@
         <v>45</v>
       </c>
       <c r="AE64" t="s" s="2">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="AF64" t="s" s="2">
         <v>43</v>
@@ -9087,7 +9080,7 @@
         <v>45</v>
       </c>
       <c r="AM64" t="s" s="2">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="AN64" t="s" s="2">
         <v>45</v>
@@ -9098,11 +9091,11 @@
     </row>
     <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B65" s="2"/>
       <c r="C65" t="s" s="2">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D65" s="2"/>
       <c r="E65" t="s" s="2">
@@ -9124,10 +9117,10 @@
         <v>101</v>
       </c>
       <c r="K65" t="s" s="2">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="L65" t="s" s="2">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="M65" t="s" s="2">
         <v>104</v>
@@ -9182,7 +9175,7 @@
         <v>45</v>
       </c>
       <c r="AE65" t="s" s="2">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="AF65" t="s" s="2">
         <v>43</v>
@@ -9217,7 +9210,7 @@
     </row>
     <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B66" s="2"/>
       <c r="C66" t="s" s="2">
@@ -9243,16 +9236,16 @@
         <v>153</v>
       </c>
       <c r="K66" t="s" s="2">
+        <v>395</v>
+      </c>
+      <c r="L66" t="s" s="2">
+        <v>396</v>
+      </c>
+      <c r="M66" t="s" s="2">
         <v>397</v>
       </c>
-      <c r="L66" t="s" s="2">
-        <v>398</v>
-      </c>
-      <c r="M66" t="s" s="2">
-        <v>399</v>
-      </c>
       <c r="N66" t="s" s="2">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="O66" t="s" s="2">
         <v>45</v>
@@ -9277,13 +9270,13 @@
         <v>45</v>
       </c>
       <c r="W66" t="s" s="2">
-        <v>169</v>
+        <v>286</v>
       </c>
       <c r="X66" t="s" s="2">
-        <v>170</v>
+        <v>398</v>
       </c>
       <c r="Y66" t="s" s="2">
-        <v>171</v>
+        <v>399</v>
       </c>
       <c r="Z66" t="s" s="2">
         <v>45</v>
@@ -9301,7 +9294,7 @@
         <v>45</v>
       </c>
       <c r="AE66" t="s" s="2">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="AF66" t="s" s="2">
         <v>55</v>
@@ -9322,13 +9315,13 @@
         <v>400</v>
       </c>
       <c r="AL66" t="s" s="2">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="AM66" t="s" s="2">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="AN66" t="s" s="2">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="AO66" t="s" s="2">
         <v>45</v>
@@ -9365,13 +9358,13 @@
         <v>402</v>
       </c>
       <c r="L67" t="s" s="2">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="M67" t="s" s="2">
         <v>403</v>
       </c>
       <c r="N67" t="s" s="2">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="O67" t="s" s="2">
         <v>45</v>
@@ -9439,16 +9432,16 @@
         <v>404</v>
       </c>
       <c r="AL67" t="s" s="2">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="AM67" t="s" s="2">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="AN67" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO67" t="s" s="2">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="68" hidden="true">
@@ -9484,13 +9477,13 @@
         <v>402</v>
       </c>
       <c r="L68" t="s" s="2">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="M68" t="s" s="2">
         <v>403</v>
       </c>
       <c r="N68" t="s" s="2">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="O68" t="s" s="2">
         <v>45</v>
@@ -9558,16 +9551,16 @@
         <v>404</v>
       </c>
       <c r="AL68" t="s" s="2">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="AM68" t="s" s="2">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="AN68" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO68" t="s" s="2">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="69" hidden="true">
@@ -9607,7 +9600,7 @@
         <v>408</v>
       </c>
       <c r="N69" t="s" s="2">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="O69" t="s" s="2">
         <v>45</v>
@@ -9632,13 +9625,13 @@
         <v>45</v>
       </c>
       <c r="W69" t="s" s="2">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="X69" t="s" s="2">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="Y69" t="s" s="2">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="Z69" t="s" s="2">
         <v>45</v>
@@ -9665,7 +9658,7 @@
         <v>55</v>
       </c>
       <c r="AH69" t="s" s="2">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="AI69" t="s" s="2">
         <v>67</v>
@@ -9680,7 +9673,7 @@
         <v>98</v>
       </c>
       <c r="AM69" t="s" s="2">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="AN69" t="s" s="2">
         <v>45</v>
@@ -9695,7 +9688,7 @@
       </c>
       <c r="B70" s="2"/>
       <c r="C70" t="s" s="2">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D70" s="2"/>
       <c r="E70" t="s" s="2">
@@ -9717,16 +9710,16 @@
         <v>153</v>
       </c>
       <c r="K70" t="s" s="2">
+        <v>254</v>
+      </c>
+      <c r="L70" t="s" s="2">
+        <v>255</v>
+      </c>
+      <c r="M70" t="s" s="2">
+        <v>256</v>
+      </c>
+      <c r="N70" t="s" s="2">
         <v>257</v>
-      </c>
-      <c r="L70" t="s" s="2">
-        <v>258</v>
-      </c>
-      <c r="M70" t="s" s="2">
-        <v>259</v>
-      </c>
-      <c r="N70" t="s" s="2">
-        <v>260</v>
       </c>
       <c r="O70" t="s" s="2">
         <v>45</v>
@@ -9751,13 +9744,13 @@
         <v>45</v>
       </c>
       <c r="W70" t="s" s="2">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="X70" t="s" s="2">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="Y70" t="s" s="2">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="Z70" t="s" s="2">
         <v>45</v>
@@ -9793,19 +9786,19 @@
         <v>45</v>
       </c>
       <c r="AK70" t="s" s="2">
+        <v>260</v>
+      </c>
+      <c r="AL70" t="s" s="2">
+        <v>261</v>
+      </c>
+      <c r="AM70" t="s" s="2">
+        <v>262</v>
+      </c>
+      <c r="AN70" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO70" t="s" s="2">
         <v>263</v>
-      </c>
-      <c r="AL70" t="s" s="2">
-        <v>264</v>
-      </c>
-      <c r="AM70" t="s" s="2">
-        <v>265</v>
-      </c>
-      <c r="AN70" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO70" t="s" s="2">
-        <v>266</v>
       </c>
     </row>
     <row r="71" hidden="true">
@@ -9842,10 +9835,10 @@
         <v>412</v>
       </c>
       <c r="M71" t="s" s="2">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="N71" t="s" s="2">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="O71" t="s" s="2">
         <v>45</v>
@@ -9915,10 +9908,10 @@
         <v>45</v>
       </c>
       <c r="AL71" t="s" s="2">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="AM71" t="s" s="2">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="AN71" t="s" s="2">
         <v>45</v>

</xml_diff>